<commit_message>
Changed question numbers in survey
</commit_message>
<xml_diff>
--- a/Iteration 1/Iteration 1 Survey/Survey_v3.xlsx
+++ b/Iteration 1/Iteration 1 Survey/Survey_v3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Personal Information</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Correct Answer</t>
+  </si>
+  <si>
+    <t>Question 7</t>
+  </si>
+  <si>
+    <t>Question 8</t>
   </si>
 </sst>
 </file>
@@ -358,14 +364,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -373,34 +417,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -413,20 +429,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,231 +1041,231 @@
       <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="22" t="s">
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="24" t="s">
+      <c r="E53" s="37"/>
+      <c r="F53" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G53" s="25"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="29" t="s">
+      <c r="G53" s="21"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="J53" s="30"/>
+      <c r="J53" s="29"/>
     </row>
     <row r="54" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A54" s="27"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="33" t="s">
+      <c r="A54" s="23"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G54" s="32" t="s">
+      <c r="G54" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H54" s="32" t="s">
+      <c r="H54" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I54" s="41" t="s">
+      <c r="I54" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J54" s="31"/>
+      <c r="J54" s="27"/>
     </row>
     <row r="55" spans="1:10" s="2" customFormat="1" ht="18.75">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="36"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="40"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
-      <c r="I56" s="28" t="s">
+      <c r="I56" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J56" s="17"/>
+      <c r="J56" s="25"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="28" t="s">
+      <c r="I57" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="J57" s="17"/>
+      <c r="J57" s="25"/>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
+      <c r="B58" s="42"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="43"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="17"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="25"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="42" t="s">
+      <c r="I59" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="J59" s="17"/>
+      <c r="J59" s="25"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="17"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="25"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="42" t="s">
+      <c r="I60" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="J60" s="17"/>
+      <c r="J60" s="25"/>
     </row>
     <row r="61" spans="1:10" ht="18.75">
-      <c r="A61" s="40" t="s">
+      <c r="A61" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
+      <c r="J61" s="43"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
-      <c r="I62" s="28" t="s">
+      <c r="I62" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="J62" s="17"/>
+      <c r="J62" s="25"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="17"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="25"/>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
-      <c r="I63" s="28" t="s">
+      <c r="I63" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J63" s="17"/>
+      <c r="J63" s="25"/>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
+      <c r="J64" s="43"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
+      <c r="A65" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="24"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
       <c r="F65" s="9"/>
       <c r="G65" s="8"/>
       <c r="H65" s="9"/>
-      <c r="I65" s="28" t="s">
+      <c r="I65" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="J65" s="17"/>
+      <c r="J65" s="25"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
+      <c r="A66" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
-      <c r="I66" s="28" t="s">
+      <c r="I66" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="J66" s="17"/>
+      <c r="J66" s="25"/>
     </row>
     <row r="68" spans="1:10" ht="18.75">
-      <c r="A68" s="45" t="s">
+      <c r="A68" s="16" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1288,7 +1294,7 @@
       <c r="J70" s="6"/>
     </row>
     <row r="71" spans="1:10" ht="18.75">
-      <c r="A71" s="46"/>
+      <c r="A71" s="17"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
@@ -1300,7 +1306,7 @@
       <c r="J71" s="6"/>
     </row>
     <row r="72" spans="1:10" ht="18.75">
-      <c r="A72" s="45"/>
+      <c r="A72" s="16"/>
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
@@ -1334,14 +1340,14 @@
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
-      <c r="G74" s="43" t="s">
+      <c r="G74" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H74" s="44"/>
-      <c r="I74" s="18" t="s">
+      <c r="H74" s="19"/>
+      <c r="I74" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="J74" s="18"/>
+      <c r="J74" s="46"/>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" s="11"/>
@@ -1349,8 +1355,8 @@
         <v>46</v>
       </c>
       <c r="H75" s="5"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="14"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="32"/>
     </row>
     <row r="76" spans="1:10">
       <c r="C76" s="11"/>
@@ -1359,8 +1365,8 @@
       </c>
       <c r="E76" s="1"/>
       <c r="H76" s="5"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="14"/>
+      <c r="I76" s="32"/>
+      <c r="J76" s="32"/>
     </row>
     <row r="77" spans="1:10">
       <c r="C77" s="11"/>
@@ -1369,8 +1375,8 @@
       </c>
       <c r="E77" s="1"/>
       <c r="H77" s="5"/>
-      <c r="I77" s="14"/>
-      <c r="J77" s="14"/>
+      <c r="I77" s="32"/>
+      <c r="J77" s="32"/>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="1" t="s">
@@ -1470,6 +1476,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="A58:J58"/>
+    <mergeCell ref="A61:J61"/>
+    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A55:J55"/>
     <mergeCell ref="G74:H74"/>
     <mergeCell ref="F53:H53"/>
     <mergeCell ref="A54:E54"/>
@@ -1486,31 +1514,9 @@
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="A57:C57"/>
     <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A55:J55"/>
-    <mergeCell ref="A58:J58"/>
-    <mergeCell ref="A61:J61"/>
-    <mergeCell ref="A64:J64"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="I75:J75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"&amp;14Navigation survey for voice controlled browsing</oddHeader>
   </headerFooter>

</xml_diff>